<commit_message>
Orden Modificacion -Bug Fixed-
</commit_message>
<xml_diff>
--- a/SOP_IAA/Plantillas/Orden_Modificacion.xlsx
+++ b/SOP_IAA/Plantillas/Orden_Modificacion.xlsx
@@ -132,7 +132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="14">
+  <numFmts count="18">
     <numFmt numFmtId="7" formatCode="&quot;₡&quot;#,##0.00_);\(&quot;₡&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;₡&quot;* #,##0.00_);_(&quot;₡&quot;* \(#,##0.00\);_(&quot;₡&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -147,6 +147,10 @@
     <numFmt numFmtId="172" formatCode="_([$₡-140A]* #,##0.00_);_([$₡-140A]* \(#,##0.00\);_([$₡-140A]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="173" formatCode="&quot;¢&quot;_(* ######\ \ ###\ \ ###.000_);[Red]&quot;¢&quot;_(* ######\ ###\ ###.000_);_(&quot;¢&quot;* &quot;0.000&quot;_);_(@_)"/>
     <numFmt numFmtId="174" formatCode="_(* #\ \ ###\ \ ###.00_);_(* #\ ###\ ###.00_);_(&quot;&quot;* &quot;0.00&quot;_);_(@_)"/>
+    <numFmt numFmtId="175" formatCode="_([$₡-140A]* #,##0.000_);_([$₡-140A]* \(#,##0.000\);_([$₡-140A]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_([$₡-140A]* #,##0.0000_);_([$₡-140A]* \(#,##0.0000\);_([$₡-140A]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="#,##0.000_);[Red]\(#,##0.000\)"/>
+    <numFmt numFmtId="178" formatCode="&quot;₡&quot;#,##0.0000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -528,7 +532,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -670,17 +674,11 @@
     <xf numFmtId="43" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="3" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="3" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -692,12 +690,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="3" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="3" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -713,14 +705,12 @@
     <xf numFmtId="43" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="172" fontId="15" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="172" fontId="15" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="169" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -752,11 +742,17 @@
     <xf numFmtId="49" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="174" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="15" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -765,17 +761,7 @@
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1150,7 +1136,7 @@
   <dimension ref="A1:AW152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1166,7 +1152,8 @@
     <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="20.85546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="2"/>
+    <col min="12" max="50" width="24.85546875" style="2" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
@@ -1284,7 +1271,7 @@
       <c r="A13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="95"/>
+      <c r="B13" s="89"/>
       <c r="C13" s="27"/>
       <c r="D13" s="27"/>
       <c r="E13" s="28"/>
@@ -1318,8 +1305,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="99"/>
-      <c r="B15" s="99"/>
+      <c r="A15" s="98"/>
+      <c r="B15" s="98"/>
       <c r="C15" s="33"/>
       <c r="D15" s="34"/>
       <c r="E15" s="35"/>
@@ -1329,10 +1316,10 @@
       <c r="I15" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="98" t="s">
+      <c r="J15" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="94"/>
+      <c r="K15" s="88"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E16" s="39"/>
@@ -1397,99 +1384,93 @@
       <c r="J19" s="55"/>
       <c r="K19" s="56"/>
     </row>
-    <row r="20" spans="1:49" s="65" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:49" s="63" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="57"/>
       <c r="B20" s="58"/>
       <c r="C20" s="59"/>
-      <c r="D20" s="96"/>
+      <c r="D20" s="90"/>
       <c r="E20" s="60"/>
       <c r="F20" s="61"/>
-      <c r="G20" s="100"/>
-      <c r="H20" s="61">
-        <f>F20-E20</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="62"/>
-      <c r="J20" s="63">
+      <c r="G20" s="93"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="62">
         <f>SUM(K20:K20)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="64"/>
-    </row>
-    <row r="21" spans="1:49" s="65" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="66"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="97"/>
+      <c r="K20" s="95"/>
+    </row>
+    <row r="21" spans="1:49" s="63" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="64"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="91"/>
       <c r="E21" s="60"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="100"/>
-      <c r="H21" s="70">
-        <f t="shared" ref="H21" si="0">F21-E21</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="71"/>
-      <c r="J21" s="63">
+      <c r="F21" s="61"/>
+      <c r="G21" s="93"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="62">
         <f>SUM(K21:K21)</f>
         <v>0</v>
       </c>
-      <c r="K21" s="64"/>
-    </row>
-    <row r="22" spans="1:49" s="78" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="72"/>
-      <c r="B22" s="72"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="75"/>
+      <c r="K21" s="95"/>
+    </row>
+    <row r="22" spans="1:49" s="74" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="68"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="71"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="76"/>
-      <c r="K22" s="77"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="73"/>
     </row>
     <row r="24" spans="1:49" ht="18" x14ac:dyDescent="0.25">
       <c r="D24" s="8"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="81"/>
-      <c r="K24" s="82"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="94"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="94"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="97"/>
     </row>
     <row r="25" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="I25" s="83" t="s">
+      <c r="I25" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="84">
+      <c r="J25" s="79">
         <f>SUM(K25:K25)</f>
         <v>0</v>
       </c>
-      <c r="K25" s="85"/>
+      <c r="K25" s="96"/>
     </row>
     <row r="26" spans="1:49" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="B26" s="86"/>
-      <c r="C26" s="86"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="80"/>
       <c r="I26" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="84">
+      <c r="J26" s="79">
         <f>SUM(K26:K26)</f>
         <v>0</v>
       </c>
-      <c r="K26" s="85"/>
+      <c r="K26" s="96"/>
     </row>
     <row r="27" spans="1:49" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="87"/>
-      <c r="C27" s="87"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
       <c r="F27" s="5"/>
       <c r="G27" s="6"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="88"/>
-      <c r="J27" s="88"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -1530,9 +1511,9 @@
       <c r="AW27" s="2"/>
     </row>
     <row r="28" spans="1:49" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="89"/>
-      <c r="B28" s="90"/>
-      <c r="C28" s="90"/>
+      <c r="A28" s="83"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="84"/>
       <c r="D28" s="3"/>
       <c r="E28" s="4"/>
       <c r="F28" s="5"/>
@@ -1581,15 +1562,15 @@
     </row>
     <row r="29" spans="1:49" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
-      <c r="B29" s="90"/>
-      <c r="C29" s="90"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="84"/>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="91"/>
+      <c r="F29" s="85"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="91"/>
-      <c r="I29" s="91"/>
-      <c r="J29" s="91"/>
+      <c r="H29" s="85"/>
+      <c r="I29" s="85"/>
+      <c r="J29" s="85"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -1631,9 +1612,9 @@
     </row>
     <row r="30" spans="1:49" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="90"/>
-      <c r="C30" s="90"/>
-      <c r="D30" s="92"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="86"/>
       <c r="E30" s="4"/>
       <c r="F30" s="5"/>
       <c r="G30" s="6"/>
@@ -1681,13 +1662,13 @@
     </row>
     <row r="31" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="93"/>
-      <c r="C31" s="93"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="87"/>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="91"/>
+      <c r="F31" s="85"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="91"/>
+      <c r="H31" s="85"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="L31" s="2"/>
@@ -1731,8 +1712,8 @@
     </row>
     <row r="32" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
-      <c r="B32" s="93"/>
-      <c r="C32" s="93"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="87"/>
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
       <c r="F32" s="5"/>
@@ -1781,8 +1762,8 @@
     </row>
     <row r="33" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
-      <c r="B33" s="93"/>
-      <c r="C33" s="93"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="87"/>
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
       <c r="F33" s="5"/>
@@ -7785,10 +7766,10 @@
     <mergeCell ref="A15:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="G20:G21">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",G20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Error">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Error">
       <formula>NOT(ISERROR(SEARCH("Error",G20)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>